<commit_message>
Updated scores not calculating correctly
</commit_message>
<xml_diff>
--- a/Lemmas.xlsx
+++ b/Lemmas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usi365-my.sharepoint.com/personal/zanari_usi_ch/Documents/PROJECTS/2023_EYR_ITICSE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie.LAPTOP-GOIIMLLB\Desktop\FYP\4th-Year-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:40000_{5E1B72D6-F849-4E53-B440-FA1C5CE0BD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA72472-FE1D-447F-8264-45F20EE97BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="3"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cat" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="436">
   <si>
     <t>knowledge</t>
   </si>
@@ -1352,7 +1352,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1433,13 +1433,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1453,7 +1453,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1471,9 +1471,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1511,7 +1511,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1617,7 +1617,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1759,14 +1759,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2012,10 +2012,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A74" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2884,18 +2884,18 @@
     <sortCondition ref="A223"/>
   </sortState>
   <conditionalFormatting sqref="A2:A172">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3040,11 +3040,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A244"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:A236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="G169" sqref="G169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,1005 +3279,965 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>390</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>362</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>412</v>
+        <v>375</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>375</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>320</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>247</v>
+        <v>360</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>360</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>224</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>413</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>347</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>203</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>422</v>
+        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>277</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>251</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>321</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>326</v>
+        <v>213</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>227</v>
+        <v>258</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>258</v>
+        <v>369</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>309</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>369</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>244</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>243</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>336</v>
+        <v>377</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>317</v>
+        <v>372</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>365</v>
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>259</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>367</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>287</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>361</v>
+        <v>403</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>403</v>
+        <v>293</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>339</v>
+        <v>218</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>218</v>
+        <v>378</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>252</v>
+        <v>278</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>378</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>278</v>
+        <v>216</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>279</v>
+        <v>391</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>391</v>
+        <v>337</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>337</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>219</v>
+        <v>404</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>404</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>84</v>
+        <v>229</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>221</v>
+        <v>414</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>180</v>
+        <v>423</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>231</v>
+        <v>280</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>414</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>423</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>280</v>
+        <v>415</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>271</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>415</v>
+        <v>319</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>226</v>
+        <v>416</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>271</v>
+        <v>405</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>319</v>
+        <v>406</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>416</v>
+        <v>306</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>318</v>
+        <v>239</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>406</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>306</v>
+        <v>260</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>239</v>
+        <v>313</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>407</v>
+        <v>240</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>212</v>
+        <v>424</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>322</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>313</v>
+        <v>241</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>240</v>
+        <v>359</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>424</v>
+        <v>379</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>322</v>
+        <v>335</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>241</v>
+        <v>298</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>359</v>
+        <v>265</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>335</v>
+        <v>266</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>266</v>
+        <v>310</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>87</v>
+        <v>381</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>292</v>
+        <v>325</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>214</v>
+        <v>308</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>380</v>
+        <v>296</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>310</v>
+        <v>374</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>381</v>
+        <v>330</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>308</v>
+        <v>267</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>30</v>
+        <v>268</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>48</v>
+        <v>333</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>374</v>
+        <v>348</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>330</v>
+        <v>261</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>332</v>
+        <v>392</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>267</v>
+        <v>334</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>281</v>
+        <v>236</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>333</v>
+        <v>254</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>348</v>
+        <v>417</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>392</v>
+        <v>197</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>334</v>
+        <v>230</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>282</v>
+        <v>352</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>236</v>
+        <v>269</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>254</v>
+        <v>368</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>417</v>
+        <v>299</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>291</v>
+        <v>393</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>197</v>
+        <v>289</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>352</v>
+        <v>262</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>269</v>
+        <v>305</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>299</v>
+        <v>418</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>393</v>
+        <v>425</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>289</v>
+        <v>304</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>272</v>
+        <v>408</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>66</v>
+        <v>386</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>262</v>
+        <v>409</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>305</v>
+        <v>357</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>340</v>
+        <v>398</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>418</v>
+        <v>354</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>425</v>
+        <v>290</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>304</v>
+        <v>263</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>408</v>
+        <v>270</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>386</v>
+        <v>426</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>409</v>
+        <v>248</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>357</v>
+        <v>311</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>354</v>
+        <v>206</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>263</v>
+        <v>419</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>270</v>
+        <v>366</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>426</v>
+        <v>284</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>248</v>
+        <v>344</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>387</v>
+        <v>427</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>283</v>
+        <v>341</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>419</v>
+        <v>204</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>284</v>
+        <v>223</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>427</v>
+        <v>300</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>220</v>
+        <v>388</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>341</v>
+        <v>235</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>204</v>
+        <v>420</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>223</v>
+        <v>329</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>355</v>
+        <v>198</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>300</v>
+        <v>353</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>388</v>
+        <v>202</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>420</v>
+        <v>295</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>370</v>
+        <v>323</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>329</v>
+        <v>303</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>198</v>
+        <v>324</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>353</v>
+        <v>382</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>285</v>
+        <v>428</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>295</v>
+        <v>383</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>323</v>
+        <v>363</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>303</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>382</v>
+        <v>301</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>208</v>
+        <v>373</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>428</v>
+        <v>384</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
         <v>431</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A307">
-    <sortCondition ref="A307"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A299">
+    <sortCondition ref="A299"/>
   </sortState>
-  <conditionalFormatting sqref="A2:A244">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  <conditionalFormatting sqref="A2:A236">
+    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>